<commit_message>
modified:   Jack/batch_test/Jack_cpp_1_0.cpp 	modified:   Jack/batch_test/jack_config.json 	modified:   Jack/batch_test/jack_test_info.xlsx 	modified:   Jack/batch_test/results.csv
</commit_message>
<xml_diff>
--- a/Jack/batch_test/jack_test_info.xlsx
+++ b/Jack/batch_test/jack_test_info.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="23190" windowHeight="8460"/>
+    <workbookView windowWidth="18585" windowHeight="18915"/>
   </bookViews>
   <sheets>
     <sheet name="6" sheetId="6" r:id="rId1"/>
-    <sheet name="7" sheetId="13" r:id="rId2"/>
-    <sheet name="4" sheetId="9" r:id="rId3"/>
-    <sheet name="5" sheetId="4" r:id="rId4"/>
-    <sheet name="7-N" sheetId="14" r:id="rId5"/>
-    <sheet name="8列炮" sheetId="3" r:id="rId6"/>
-    <sheet name="奇蛇-N" sheetId="15" r:id="rId7"/>
-    <sheet name="5列炮" sheetId="11" r:id="rId8"/>
-    <sheet name="6-2" sheetId="1" r:id="rId9"/>
+    <sheet name="6-2" sheetId="1" r:id="rId2"/>
+    <sheet name="7" sheetId="13" r:id="rId3"/>
+    <sheet name="4" sheetId="9" r:id="rId4"/>
+    <sheet name="5" sheetId="4" r:id="rId5"/>
+    <sheet name="7-N" sheetId="14" r:id="rId6"/>
+    <sheet name="8列炮" sheetId="3" r:id="rId7"/>
+    <sheet name="奇蛇-N" sheetId="15" r:id="rId8"/>
+    <sheet name="5列炮" sheetId="11" r:id="rId9"/>
     <sheet name="9-2" sheetId="12" r:id="rId10"/>
     <sheet name="9" sheetId="5" r:id="rId11"/>
     <sheet name="3" sheetId="10" r:id="rId12"/>
@@ -44,7 +44,7 @@
     <t>小丑类型</t>
   </si>
   <si>
-    <t>早爆</t>
+    <t>全部</t>
   </si>
   <si>
     <t>输出植物信息</t>
@@ -64,7 +64,7 @@
     <t>地图类型</t>
   </si>
   <si>
-    <t>后院</t>
+    <t>前院</t>
   </si>
   <si>
     <t>植物列数</t>
@@ -88,7 +88,7 @@
     <t>被炸情况</t>
   </si>
   <si>
-    <t>下炸上</t>
+    <t>上炸下</t>
   </si>
   <si>
     <t>曾</t>
@@ -157,6 +157,12 @@
     <t>晚爆</t>
   </si>
   <si>
+    <t>后院</t>
+  </si>
+  <si>
+    <t>下炸上</t>
+  </si>
+  <si>
     <t>非永动</t>
   </si>
   <si>
@@ -166,16 +172,10 @@
     <t>炮</t>
   </si>
   <si>
-    <t>全部</t>
-  </si>
-  <si>
     <t>屋顶</t>
   </si>
   <si>
-    <t>上炸下</t>
-  </si>
-  <si>
-    <t>前院</t>
+    <t>早爆</t>
   </si>
   <si>
     <t>正炸</t>
@@ -1094,13 +1094,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/customStorage/customStorage.xml><?xml version="1.0" encoding="utf-8"?>
-<customStorage xmlns="https://web.wps.cn/et/2018/main">
-  <book/>
-  <sheets/>
-</customStorage>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="WPS">
   <a:themeElements>
@@ -1353,8 +1346,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
@@ -1442,9 +1435,7 @@
       <c r="G3" s="3">
         <v>1</v>
       </c>
-      <c r="I3" s="3">
-        <v>783</v>
-      </c>
+      <c r="I3" s="3"/>
       <c r="K3" s="3"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -1466,7 +1457,7 @@
         <v>17</v>
       </c>
       <c r="G4" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="3"/>
       <c r="K4" s="3"/>
@@ -1523,7 +1514,7 @@
     </row>
     <row r="7" spans="4:14">
       <c r="D7" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>23</v>
@@ -1532,7 +1523,7 @@
         <v>17</v>
       </c>
       <c r="G7" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="3"/>
       <c r="K7" s="3"/>
@@ -1556,7 +1547,7 @@
         <v>17</v>
       </c>
       <c r="G8" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="3"/>
       <c r="K8" s="3"/>
@@ -1578,7 +1569,7 @@
         <v>25</v>
       </c>
       <c r="B10" s="3">
-        <v>2000000</v>
+        <v>100000</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -1872,7 +1863,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -1896,7 +1887,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -1924,7 +1915,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3">
         <v>9</v>
@@ -1933,7 +1924,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G3" s="3">
         <v>1</v>
@@ -1959,7 +1950,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
@@ -1983,7 +1974,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -2025,7 +2016,7 @@
         <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -2156,7 +2147,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -2372,7 +2363,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -2396,7 +2387,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -2424,7 +2415,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3">
         <v>9</v>
@@ -2433,7 +2424,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G3" s="3">
         <v>1</v>
@@ -2459,7 +2450,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
@@ -2483,7 +2474,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -2525,7 +2516,7 @@
         <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -2656,7 +2647,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -2871,7 +2862,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -2895,7 +2886,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -2923,7 +2914,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3">
         <v>6</v>
@@ -2932,7 +2923,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -3362,7 +3353,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -3386,7 +3377,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -3414,7 +3405,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3">
         <v>5</v>
@@ -3845,6 +3836,502 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr codeName="Sheet13"/>
+  <dimension ref="A1:N25"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33333333333333" style="1"/>
+    <col min="3" max="8" width="9.16666666666667" style="1"/>
+    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.16666666666667" style="1"/>
+    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.16666666666667" style="1"/>
+    <col min="13" max="13" width="11.3333333333333" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.16666666666667" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:14">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="I1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="2"/>
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:14">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="M2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" spans="1:14">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="3">
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3">
+        <v>300</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" s="1" customFormat="1" spans="1:14">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="3">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" s="1" customFormat="1" spans="1:14">
+      <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="3">
+        <v>4</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" s="1" customFormat="1" spans="1:14">
+      <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" s="1" customFormat="1" spans="4:14">
+      <c r="D7" s="3">
+        <v>3</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" s="1" customFormat="1" spans="1:14">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>4</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" s="1" customFormat="1" spans="4:14">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" s="1" customFormat="1" spans="1:14">
+      <c r="A10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="3">
+        <v>100000</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" s="1" customFormat="1" spans="1:14">
+      <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" s="1" customFormat="1" spans="4:14">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" s="1" customFormat="1" spans="1:14">
+      <c r="A13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="3">
+        <v>8000</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" s="1" customFormat="1" spans="1:14">
+      <c r="A14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="2">
+        <v>3000</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" s="1" customFormat="1" spans="1:14">
+      <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" s="1" customFormat="1" spans="1:14">
+      <c r="A16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" s="1" customFormat="1" spans="4:14">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" s="1" customFormat="1" spans="1:14">
+      <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" s="1" customFormat="1" spans="1:14">
+      <c r="A19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" s="1" customFormat="1" spans="1:14">
+      <c r="A20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="3">
+        <v>100</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" s="1" customFormat="1" spans="1:14">
+      <c r="A21" s="2"/>
+      <c r="B21" s="3">
+        <v>100</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" s="1" customFormat="1" spans="4:14">
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" s="1" customFormat="1" spans="1:14">
+      <c r="A23"/>
+      <c r="B23"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" s="1" customFormat="1" spans="1:14">
+      <c r="A24"/>
+      <c r="B24"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+    </row>
+    <row r="25" s="1" customFormat="1" spans="4:14">
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="K1:K2"/>
+  </mergeCells>
+  <dataValidations count="12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>"全部,早爆,晚爆"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>"前院,后院,屋顶"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+      <formula1>"上炸下,下炸上,正炸"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
+      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+      <formula1>"南瓜,普通,炮"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+      <formula1>"通常波,旗帜波"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+      <formula1>"是,否"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+      <formula1>"卡,炮"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
+      <formula1>"随机,最快,最慢"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
+      <formula1>"曾,喷"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
+      <formula1>"永动,非永动"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet35"/>
   <dimension ref="A1:N25"/>
@@ -3896,7 +4383,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -3924,7 +4411,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3">
         <v>9</v>
@@ -3933,7 +4420,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -4023,7 +4510,7 @@
         <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -4096,7 +4583,7 @@
         <v>26</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -4154,7 +4641,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -4342,7 +4829,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet34"/>
   <dimension ref="A1:N25"/>
@@ -4370,7 +4857,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -4394,7 +4881,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -4422,7 +4909,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3">
         <v>6</v>
@@ -4594,7 +5081,7 @@
         <v>26</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -4840,7 +5327,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N25"/>
@@ -4868,7 +5355,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -4892,7 +5379,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -4920,7 +5407,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="D3" s="3">
         <v>6</v>
@@ -5092,7 +5579,7 @@
         <v>26</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -5338,7 +5825,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N25"/>
@@ -5370,7 +5857,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -5394,7 +5881,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -5422,7 +5909,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3">
         <v>8</v>
@@ -5834,7 +6321,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet48"/>
   <dimension ref="A1:N25"/>
@@ -5861,7 +6348,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -5885,7 +6372,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -5963,7 +6450,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -6137,7 +6624,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -6325,7 +6812,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:N25"/>
@@ -6353,7 +6840,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -6377,7 +6864,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -6817,7 +7304,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:N25"/>
@@ -6845,7 +7332,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -6869,7 +7356,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -6947,7 +7434,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -7129,7 +7616,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -7315,496 +7802,4 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet13"/>
-  <dimension ref="A1:N25"/>
-  <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:B19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33333333333333" style="1"/>
-    <col min="3" max="8" width="9.16666666666667" style="1"/>
-    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.16666666666667" style="1"/>
-    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.16666666666667" style="1"/>
-    <col min="13" max="13" width="11.3333333333333" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.16666666666667" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="I1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="M2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="3">
-        <v>6</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="3">
-        <v>1</v>
-      </c>
-      <c r="I3" s="3">
-        <v>300</v>
-      </c>
-      <c r="K3" s="3"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="3">
-        <v>6</v>
-      </c>
-      <c r="D4" s="3">
-        <v>5</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0</v>
-      </c>
-      <c r="I4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="3">
-        <v>4</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="3">
-        <v>3</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="I6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-    </row>
-    <row r="7" spans="4:14">
-      <c r="D7" s="3">
-        <v>5</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="3">
-        <v>1</v>
-      </c>
-      <c r="I7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3">
-        <v>4</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="3">
-        <v>1</v>
-      </c>
-      <c r="I8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-    </row>
-    <row r="9" spans="4:14">
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="3">
-        <v>10000000</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-    </row>
-    <row r="12" spans="4:14">
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="3">
-        <v>3200</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="A14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="2">
-        <v>3000</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="3">
-        <v>0</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-    </row>
-    <row r="17" spans="4:14">
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-    </row>
-    <row r="18" spans="1:14">
-      <c r="A18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-    </row>
-    <row r="19" spans="1:14">
-      <c r="A19" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-    </row>
-    <row r="20" spans="1:14">
-      <c r="A20" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="3">
-        <v>100</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21" s="2"/>
-      <c r="B21" s="3">
-        <v>100</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-    </row>
-    <row r="22" spans="4:14">
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-    </row>
-    <row r="23" spans="4:14">
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-    </row>
-    <row r="24" spans="4:14">
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-    </row>
-    <row r="25" spans="4:14">
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="K1:K2"/>
-  </mergeCells>
-  <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>"全部,早爆,晚爆"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>"前院,后院,屋顶"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
-      <formula1>"上炸下,下炸上,正炸"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
-      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
-      <formula1>"南瓜,普通,炮"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
-      <formula1>"通常波,旗帜波"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
-      <formula1>"是,否"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
-      <formula1>"卡,炮"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
-      <formula1>"随机,最快,最慢"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
-      <formula1>"曾,喷"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
-      <formula1>"永动,非永动"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
 </file>
</xml_diff>